<commit_message>
Latest changes updated - RahulR
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/EndToEnd.xlsx
+++ b/src/test/java/gfl/testData/EndToEnd.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>TC0042</t>
   </si>
@@ -109,12 +109,163 @@
   </si>
   <si>
     <t>UCN 10054</t>
+  </si>
+  <si>
+    <t>QvDlJ_0104807</t>
+  </si>
+  <si>
+    <t>GxzuRJLKAE</t>
+  </si>
+  <si>
+    <t>UCN 10059</t>
+  </si>
+  <si>
+    <t>hkGuI_0104208</t>
+  </si>
+  <si>
+    <t>VIqwCLtLch</t>
+  </si>
+  <si>
+    <t>UCN 10060</t>
+  </si>
+  <si>
+    <t>TSvkj_0104465</t>
+  </si>
+  <si>
+    <t>lASbruVSfm</t>
+  </si>
+  <si>
+    <t>UCN 10061</t>
+  </si>
+  <si>
+    <t>lgTuN_0104652</t>
+  </si>
+  <si>
+    <t>ylPicrFUQO</t>
+  </si>
+  <si>
+    <t>UCN 10062</t>
+  </si>
+  <si>
+    <t>fkOWM_0104632</t>
+  </si>
+  <si>
+    <t>TLzteMFtiQ</t>
+  </si>
+  <si>
+    <t>UCN 10063</t>
+  </si>
+  <si>
+    <t>dqveX_0104472</t>
+  </si>
+  <si>
+    <t>KjBQrptNsE</t>
+  </si>
+  <si>
+    <t>UCN 10064</t>
+  </si>
+  <si>
+    <t>CHVAOPODAEDZ</t>
+  </si>
+  <si>
+    <t>xlztl_0104335</t>
+  </si>
+  <si>
+    <t>nOJBSdwQys</t>
+  </si>
+  <si>
+    <t>UCN 10065</t>
+  </si>
+  <si>
+    <t>SAXlH_0104181</t>
+  </si>
+  <si>
+    <t>TwkQomKahu</t>
+  </si>
+  <si>
+    <t>UCN 10066</t>
+  </si>
+  <si>
+    <t>ZppMx_0104638</t>
+  </si>
+  <si>
+    <t>LbslEaArTy</t>
+  </si>
+  <si>
+    <t>UCN 10067</t>
+  </si>
+  <si>
+    <t>ATEZUBVGSJWU</t>
+  </si>
+  <si>
+    <t>bOmWB_0204495</t>
+  </si>
+  <si>
+    <t>hZADbpUStr</t>
+  </si>
+  <si>
+    <t>UCN 10074</t>
+  </si>
+  <si>
+    <t>sFTQS_0204575</t>
+  </si>
+  <si>
+    <t>WGBrmPNobE</t>
+  </si>
+  <si>
+    <t>UCN 10075</t>
+  </si>
+  <si>
+    <t>EBRro_0204411</t>
+  </si>
+  <si>
+    <t>MByHZ_0204288</t>
+  </si>
+  <si>
+    <t>NBxXjPmMKj</t>
+  </si>
+  <si>
+    <t>UCN 10077</t>
+  </si>
+  <si>
+    <t>ENDQl_0204408</t>
+  </si>
+  <si>
+    <t>wuXCqdhRbz</t>
+  </si>
+  <si>
+    <t>UCN 10078</t>
+  </si>
+  <si>
+    <t>fCmqd_0204236</t>
+  </si>
+  <si>
+    <t>BORZNkgKZQ</t>
+  </si>
+  <si>
+    <t>UCN 10079</t>
+  </si>
+  <si>
+    <t>YqYDo_0204865</t>
+  </si>
+  <si>
+    <t>DtAkiAElrd</t>
+  </si>
+  <si>
+    <t>zNxDy_0204774</t>
+  </si>
+  <si>
+    <t>SPiEJFAeIZ</t>
+  </si>
+  <si>
+    <t>UCN 10081</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -468,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,7 +627,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O1048564"/>
+  <dimension ref="A1:S1048564"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
@@ -484,16 +635,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -551,10 +702,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>21</v>
@@ -584,10 +735,13 @@
         <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="O2" t="s">
         <v>7</v>
+      </c>
+      <c r="S2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="1048564" spans="1:1">

</xml_diff>

<commit_message>
- Adding Driver Name - Updating driver notes by comma - Adding Dispatcher Name - Added interface for the Excel Column constants
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/EndToEnd.xlsx
+++ b/src/test/java/gfl/testData/EndToEnd.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\GFL\WISHES\gflwishes\src\test\java\gfl\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9395318-73CC-4581-9DF3-EB7CF878CF5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16890" windowHeight="5490"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>TC0042</t>
   </si>
@@ -51,12 +57,6 @@
     <t>17 PARRY RD,AJAX, ONTARIO L1S 1R1</t>
   </si>
   <si>
-    <t>mXgvi_3103424</t>
-  </si>
-  <si>
-    <t>sBBmAGjVlg</t>
-  </si>
-  <si>
     <t>Material</t>
   </si>
   <si>
@@ -96,9 +96,6 @@
     <t>COMPLETED</t>
   </si>
   <si>
-    <t>Roshan's VAN</t>
-  </si>
-  <si>
     <t>Roshan Masood</t>
   </si>
   <si>
@@ -108,192 +105,6 @@
     <t>Shubhi Gupta</t>
   </si>
   <si>
-    <t>UCN 10054</t>
-  </si>
-  <si>
-    <t>QvDlJ_0104807</t>
-  </si>
-  <si>
-    <t>GxzuRJLKAE</t>
-  </si>
-  <si>
-    <t>UCN 10059</t>
-  </si>
-  <si>
-    <t>hkGuI_0104208</t>
-  </si>
-  <si>
-    <t>VIqwCLtLch</t>
-  </si>
-  <si>
-    <t>UCN 10060</t>
-  </si>
-  <si>
-    <t>TSvkj_0104465</t>
-  </si>
-  <si>
-    <t>lASbruVSfm</t>
-  </si>
-  <si>
-    <t>UCN 10061</t>
-  </si>
-  <si>
-    <t>lgTuN_0104652</t>
-  </si>
-  <si>
-    <t>ylPicrFUQO</t>
-  </si>
-  <si>
-    <t>UCN 10062</t>
-  </si>
-  <si>
-    <t>fkOWM_0104632</t>
-  </si>
-  <si>
-    <t>TLzteMFtiQ</t>
-  </si>
-  <si>
-    <t>UCN 10063</t>
-  </si>
-  <si>
-    <t>dqveX_0104472</t>
-  </si>
-  <si>
-    <t>KjBQrptNsE</t>
-  </si>
-  <si>
-    <t>UCN 10064</t>
-  </si>
-  <si>
-    <t>CHVAOPODAEDZ</t>
-  </si>
-  <si>
-    <t>xlztl_0104335</t>
-  </si>
-  <si>
-    <t>nOJBSdwQys</t>
-  </si>
-  <si>
-    <t>UCN 10065</t>
-  </si>
-  <si>
-    <t>SAXlH_0104181</t>
-  </si>
-  <si>
-    <t>TwkQomKahu</t>
-  </si>
-  <si>
-    <t>UCN 10066</t>
-  </si>
-  <si>
-    <t>ZppMx_0104638</t>
-  </si>
-  <si>
-    <t>LbslEaArTy</t>
-  </si>
-  <si>
-    <t>UCN 10067</t>
-  </si>
-  <si>
-    <t>ATEZUBVGSJWU</t>
-  </si>
-  <si>
-    <t>bOmWB_0204495</t>
-  </si>
-  <si>
-    <t>hZADbpUStr</t>
-  </si>
-  <si>
-    <t>UCN 10074</t>
-  </si>
-  <si>
-    <t>sFTQS_0204575</t>
-  </si>
-  <si>
-    <t>WGBrmPNobE</t>
-  </si>
-  <si>
-    <t>UCN 10075</t>
-  </si>
-  <si>
-    <t>EBRro_0204411</t>
-  </si>
-  <si>
-    <t>MByHZ_0204288</t>
-  </si>
-  <si>
-    <t>NBxXjPmMKj</t>
-  </si>
-  <si>
-    <t>UCN 10077</t>
-  </si>
-  <si>
-    <t>ENDQl_0204408</t>
-  </si>
-  <si>
-    <t>wuXCqdhRbz</t>
-  </si>
-  <si>
-    <t>UCN 10078</t>
-  </si>
-  <si>
-    <t>fCmqd_0204236</t>
-  </si>
-  <si>
-    <t>BORZNkgKZQ</t>
-  </si>
-  <si>
-    <t>UCN 10079</t>
-  </si>
-  <si>
-    <t>YqYDo_0204865</t>
-  </si>
-  <si>
-    <t>DtAkiAElrd</t>
-  </si>
-  <si>
-    <t>zNxDy_0204774</t>
-  </si>
-  <si>
-    <t>SPiEJFAeIZ</t>
-  </si>
-  <si>
-    <t>UCN 10081</t>
-  </si>
-  <si>
-    <t>dzoXD_0204347</t>
-  </si>
-  <si>
-    <t>nnyrdvMqON</t>
-  </si>
-  <si>
-    <t>lDWyd_0204693</t>
-  </si>
-  <si>
-    <t>hhyiWwaLQn</t>
-  </si>
-  <si>
-    <t>UCN 10084</t>
-  </si>
-  <si>
-    <t>GZnwF_0204214</t>
-  </si>
-  <si>
-    <t>yQCsimZPED</t>
-  </si>
-  <si>
-    <t>UCN 10085</t>
-  </si>
-  <si>
-    <t>AbdXF_0204365</t>
-  </si>
-  <si>
-    <t>IXffQkYrrj</t>
-  </si>
-  <si>
-    <t>UCN 10086</t>
-  </si>
-  <si>
     <t>KEOah_0204768</t>
   </si>
   <si>
@@ -303,21 +114,23 @@
     <t>UCN 10087</t>
   </si>
   <si>
-    <t>V_HJIRMXUJ</t>
-  </si>
-  <si>
-    <t>V_DZQHOFRS</t>
-  </si>
-  <si>
     <t>V_GBZOECUU</t>
+  </si>
+  <si>
+    <t>Scale Ticket</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Payment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -476,7 +289,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -670,35 +483,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S1048564"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R1048564"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="40" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -712,31 +525,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>4</v>
@@ -744,8 +557,17 @@
       <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -753,49 +575,46 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
       <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
         <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>93</v>
       </c>
       <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="S2" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="1048564" spans="1:1">
+    <row r="1048564" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1048564" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
- ExcelUtils change for the vehicles
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/EndToEnd.xlsx
+++ b/src/test/java/gfl/testData/EndToEnd.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\GFL\WISHES\gflwishes\src\test\java\gfl\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBACC96A-563B-49C5-80FD-E70554FA8D78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+  <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -19,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
-  <si>
-    <t>TC0042</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CustomerName</t>
   </si>
@@ -96,51 +99,15 @@
     <t>Payment</t>
   </si>
   <si>
-    <t>V_VXCHJARO</t>
-  </si>
-  <si>
-    <t>Dvrsf_0904143</t>
-  </si>
-  <si>
-    <t>tWtnqyApAI</t>
-  </si>
-  <si>
-    <t>UCN 10008</t>
-  </si>
-  <si>
-    <t>fVisK_0904487</t>
-  </si>
-  <si>
-    <t>LmEfijEnmR</t>
-  </si>
-  <si>
-    <t>UCN 10009</t>
-  </si>
-  <si>
-    <t>HXZRB_0904493</t>
-  </si>
-  <si>
-    <t>NlYEm_0904952</t>
-  </si>
-  <si>
-    <t>oXOYP_0904480</t>
-  </si>
-  <si>
-    <t>RfawTRUtHU</t>
-  </si>
-  <si>
-    <t>UCN 10011</t>
-  </si>
-  <si>
-    <t>ECRQn_0904278</t>
+    <t>V_BURCHRMM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -299,7 +266,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -500,14 +467,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R1048564"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="40.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
@@ -522,239 +487,83 @@
     <col min="15" max="15" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
         <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1048564" spans="1:1">
-      <c r="A1048564" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Working on RODSP06 Test Cases
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/EndToEnd.xlsx
+++ b/src/test/java/gfl/testData/EndToEnd.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>CustomerName</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>V_BURCHRMM</t>
+  </si>
+  <si>
+    <t>V_UWZYFESK</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
automation script for admin
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/EndToEnd.xlsx
+++ b/src/test/java/gfl/testData/EndToEnd.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>CustomerName</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>V_UWZYFESK</t>
+  </si>
+  <si>
+    <t>V_RUFSDRSN</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added new test cases for the QA-3
</commit_message>
<xml_diff>
--- a/src/test/java/gfl/testData/EndToEnd.xlsx
+++ b/src/test/java/gfl/testData/EndToEnd.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>CustomerName</t>
   </si>
@@ -102,7 +102,34 @@
     <t>V_BURCHRMM</t>
   </si>
   <si>
-    <t>V_UWZYFESK</t>
+    <t>V_RYORJHML</t>
+  </si>
+  <si>
+    <t>vBkUd_2704159</t>
+  </si>
+  <si>
+    <t>cgeIemXoBW</t>
+  </si>
+  <si>
+    <t>djGnr_2704193</t>
+  </si>
+  <si>
+    <t>fglkNGjWFg</t>
+  </si>
+  <si>
+    <t>UCN 10415</t>
+  </si>
+  <si>
+    <t>RbcLd_2704732</t>
+  </si>
+  <si>
+    <t>USDNexnDLd</t>
+  </si>
+  <si>
+    <t>UCN 10417</t>
+  </si>
+  <si>
+    <t>jDIubtQImU</t>
   </si>
 </sst>
 </file>
@@ -553,6 +580,12 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
@@ -564,6 +597,15 @@
       </c>
       <c r="I2" t="s">
         <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
       </c>
       <c r="O2" t="s">
         <v>6</v>

</xml_diff>